<commit_message>
Move event reconcile and effort data status methods to separate service classes; rewrite importer to use instantiated object with instance methods; automate matching and participant creation after effort import; rework matching methods; change name of event.first_start_time to event.start_time; change name of split.kind enum from 'waypoint' to 'intermediate'; add strip_attributes gem and related rspec; fix bug that prevented participants with 0 efforts from being found in participant search; change segment model to raise if segments are not provided in proper order; modify SetOperations module to handle blank scopes.
</commit_message>
<xml_diff>
--- a/baddata2015test.xlsx
+++ b/baddata2015test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mark/Development/OpenSplitTime/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmo/Development/OpenSplitTime/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,6 +19,9 @@
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>first_name</t>
   </si>
@@ -170,12 +173,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Got</t>
-  </si>
-  <si>
-    <t>Chicked</t>
-  </si>
-  <si>
     <t>Another</t>
   </si>
   <si>
@@ -197,12 +194,6 @@
     <t>French-Dude</t>
   </si>
   <si>
-    <t>Local</t>
-  </si>
-  <si>
-    <t>Boy</t>
-  </si>
-  <si>
     <t>Missing</t>
   </si>
   <si>
@@ -210,12 +201,24 @@
   </si>
   <si>
     <t>Backward</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Hour</t>
+  </si>
+  <si>
+    <t>Half-Hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[h]:mm:ss;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -251,10 +254,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +540,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,13 +650,13 @@
         <v>7.8472222222222221E-2</v>
       </c>
       <c r="J3" s="1">
-        <v>7.8472222222222221E-2</v>
+        <v>0.4458333333333333</v>
       </c>
       <c r="K3" s="1">
-        <v>0.86249999999999993</v>
+        <v>0.44861111111111113</v>
       </c>
       <c r="L3" s="1">
-        <v>0.8652777777777777</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="M3" s="1">
         <v>0.93125000000000002</v>
@@ -668,10 +670,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -695,30 +697,30 @@
         <v>8.4027777777777771E-2</v>
       </c>
       <c r="J4" s="1">
-        <v>8.4027777777777771E-2</v>
+        <v>0.52986111111111112</v>
       </c>
       <c r="K4" s="1">
-        <v>0.94652777777777775</v>
+        <v>0.53125</v>
       </c>
       <c r="L4" s="1">
-        <v>0.94791666666666663</v>
-      </c>
-      <c r="M4" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="M4" s="1">
         <v>0.84861111111111109</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>0.84861111111111109</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>1.0729166666666667</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -744,15 +746,15 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1">
-        <v>0.97361111111111109</v>
-      </c>
-      <c r="M5" s="2">
+        <v>0.7944444444444444</v>
+      </c>
+      <c r="M5" s="1">
         <v>1.0631944444444443</v>
       </c>
-      <c r="N5" s="2">
+      <c r="N5" s="1">
         <v>1.0638888888888889</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>1.117361111111111</v>
       </c>
     </row>
@@ -785,30 +787,30 @@
         <v>8.4027777777777771E-2</v>
       </c>
       <c r="J6" s="1">
-        <v>8.4027777777777771E-2</v>
+        <v>0.56527777777777777</v>
       </c>
       <c r="K6" s="1">
-        <v>0.9819444444444444</v>
+        <v>0.56874999999999998</v>
       </c>
       <c r="L6" s="1">
-        <v>0.98541666666666661</v>
-      </c>
-      <c r="M6" s="2">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="M6" s="1">
         <v>1.0763888888888888</v>
       </c>
-      <c r="N6" s="2">
+      <c r="N6" s="1">
         <v>1.0770833333333334</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>1.1270833333333334</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -826,36 +828,36 @@
         <v>30</v>
       </c>
       <c r="H7" s="1">
-        <v>0</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="I7" s="1">
         <v>0.11944444444444445</v>
       </c>
       <c r="J7" s="1">
-        <v>0.11944444444444445</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1.5520833333333333</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1.5625</v>
-      </c>
-      <c r="M7" s="2">
+        <v>1.1354166666666667</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.1458333333333333</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1.4590277777777778</v>
+      </c>
+      <c r="M7" s="1">
         <v>1.7236111111111112</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="1">
         <v>1.73125</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>1.8305555555555555</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -879,30 +881,30 @@
         <v>0.11805555555555557</v>
       </c>
       <c r="J8" s="1">
-        <v>0.11805555555555557</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1.5625</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1.5729166666666667</v>
-      </c>
-      <c r="M8" s="2">
+        <v>1.1458333333333333</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1.15625</v>
+      </c>
+      <c r="L8" s="1">
+        <v>1.4722222222222223</v>
+      </c>
+      <c r="M8" s="1">
         <v>1.7229166666666667</v>
       </c>
-      <c r="N8" s="2">
+      <c r="N8" s="1">
         <v>1.7249999999999999</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <v>1.8319444444444446</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -926,27 +928,27 @@
         <v>0.12916666666666668</v>
       </c>
       <c r="J9" s="1">
-        <v>0.12916666666666668</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1.6229166666666668</v>
-      </c>
-      <c r="L9" s="2">
-        <v>1.6319444444444444</v>
-      </c>
-      <c r="M9" s="2">
+        <v>1.20625</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.2152777777777779</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.5569444444444445</v>
+      </c>
+      <c r="M9" s="1">
         <v>1.7944444444444445</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="1">
         <v>1.7958333333333334</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="1">
         <v>1.8965277777777778</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -970,25 +972,21 @@
         <v>0.12847222222222224</v>
       </c>
       <c r="J10" s="1">
-        <v>0.12847222222222224</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1.6416666666666666</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2">
+        <v>1.2249999999999999</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
+        <v>1.3979166666666665</v>
+      </c>
+      <c r="M10" s="1">
         <v>1.8090277777777777</v>
       </c>
-      <c r="N10" s="2">
-        <v>1.8138888888888889</v>
-      </c>
-      <c r="O10" s="2">
-        <v>1.9048611111111111</v>
-      </c>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -1012,30 +1010,30 @@
         <v>0.12847222222222224</v>
       </c>
       <c r="J11" s="1">
-        <v>0.12847222222222224</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1.7333333333333334</v>
-      </c>
-      <c r="L11" s="2">
-        <v>1.7388888888888889</v>
-      </c>
-      <c r="M11" s="2">
+        <v>1.3166666666666667</v>
+      </c>
+      <c r="K11" s="1">
+        <v>1.3222222222222222</v>
+      </c>
+      <c r="L11" s="1">
+        <v>1.5972222222222223</v>
+      </c>
+      <c r="M11" s="1">
         <v>1.9152777777777779</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="1">
         <v>1.9166666666666667</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O11" s="1">
         <v>1.9993055555555557</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -1059,24 +1057,25 @@
         <v>0.11666666666666665</v>
       </c>
       <c r="J12" s="1">
-        <v>0.11666666666666665</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1.7138888888888888</v>
-      </c>
-      <c r="L12" s="2">
-        <v>1.7222222222222223</v>
-      </c>
-      <c r="M12" s="2">
+        <v>1.2972222222222223</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1.3055555555555556</v>
+      </c>
+      <c r="L12" s="1">
+        <v>1.5722222222222222</v>
+      </c>
+      <c r="M12" s="1">
         <v>1.8993055555555556</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="1">
         <v>1.8993055555555556</v>
       </c>
+      <c r="O12" s="1"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>57</v>
@@ -1097,26 +1096,23 @@
         <v>135</v>
       </c>
       <c r="H13" s="1">
-        <v>0</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="I13" s="1">
         <v>0.12847222222222224</v>
       </c>
       <c r="J13" s="1">
-        <v>0.12847222222222224</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="L13" s="2">
-        <v>1.8041666666666665</v>
-      </c>
-      <c r="M13" s="2">
-        <v>1.95</v>
-      </c>
-      <c r="N13" s="2">
-        <v>1.95</v>
-      </c>
+        <v>1.3833333333333335</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.3875</v>
+      </c>
+      <c r="L13" s="1">
+        <v>1.6888888888888889</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1147,20 +1143,17 @@
         <v>0.12847222222222224</v>
       </c>
       <c r="J14" s="1">
-        <v>0.12847222222222224</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1.7541666666666667</v>
-      </c>
-      <c r="L14" s="2">
-        <v>1.7562499999999999</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1.9284722222222221</v>
-      </c>
-      <c r="N14" s="2">
-        <v>1.9291666666666665</v>
-      </c>
+        <v>1.3375000000000001</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.3395833333333333</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1.715972222222222</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1187,6 +1180,11 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>